<commit_message>
made pcb in Eagle
</commit_message>
<xml_diff>
--- a/eagle/footprint_calc.xlsx
+++ b/eagle/footprint_calc.xlsx
@@ -505,7 +505,7 @@
   <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,7 +587,7 @@
         <v>-2.42</v>
       </c>
       <c r="C9" s="1">
-        <f>B9*sc</f>
+        <f t="shared" ref="C9:C16" si="0">B9*sc</f>
         <v>-95.275590551181097</v>
       </c>
     </row>
@@ -600,7 +600,7 @@
         <v>12.58</v>
       </c>
       <c r="C10" s="1">
-        <f>B10*sc</f>
+        <f t="shared" si="0"/>
         <v>495.2755905511811</v>
       </c>
     </row>
@@ -613,7 +613,7 @@
         <v>-1.92</v>
       </c>
       <c r="C11" s="1">
-        <f>B11*sc</f>
+        <f t="shared" si="0"/>
         <v>-75.590551181102356</v>
       </c>
     </row>
@@ -626,7 +626,7 @@
         <v>12.08</v>
       </c>
       <c r="C12" s="1">
-        <f>B12*sc</f>
+        <f t="shared" si="0"/>
         <v>475.5905511811024</v>
       </c>
     </row>
@@ -639,7 +639,7 @@
         <v>-3.42</v>
       </c>
       <c r="C13" s="1">
-        <f>B13*sc</f>
+        <f t="shared" si="0"/>
         <v>-134.64566929133858</v>
       </c>
     </row>
@@ -652,7 +652,7 @@
         <v>13.58</v>
       </c>
       <c r="C14" s="1">
-        <f>B14*sc</f>
+        <f t="shared" si="0"/>
         <v>534.64566929133855</v>
       </c>
     </row>
@@ -665,7 +665,7 @@
         <v>-2.92</v>
       </c>
       <c r="C15" s="1">
-        <f>B15*sc</f>
+        <f t="shared" si="0"/>
         <v>-114.96062992125984</v>
       </c>
     </row>
@@ -678,7 +678,7 @@
         <v>13.08</v>
       </c>
       <c r="C16" s="1">
-        <f>B16*sc</f>
+        <f t="shared" si="0"/>
         <v>514.96062992125985</v>
       </c>
     </row>
@@ -739,7 +739,7 @@
         <v>-17.48</v>
       </c>
       <c r="C23" s="1">
-        <f>B23*sc</f>
+        <f t="shared" ref="C23:C30" si="1">B23*sc</f>
         <v>-688.18897637795283</v>
       </c>
     </row>
@@ -752,7 +752,7 @@
         <v>32.72</v>
       </c>
       <c r="C24" s="1">
-        <f>B24*sc</f>
+        <f t="shared" si="1"/>
         <v>1288.1889763779527</v>
       </c>
     </row>
@@ -765,7 +765,7 @@
         <v>-1.88</v>
       </c>
       <c r="C25" s="1">
-        <f>B25*sc</f>
+        <f t="shared" si="1"/>
         <v>-74.015748031496059</v>
       </c>
     </row>
@@ -778,7 +778,7 @@
         <v>17.12</v>
       </c>
       <c r="C26" s="1">
-        <f>B26*sc</f>
+        <f t="shared" si="1"/>
         <v>674.01574803149617</v>
       </c>
     </row>
@@ -791,7 +791,7 @@
         <v>-18.48</v>
       </c>
       <c r="C27" s="1">
-        <f>B27*sc</f>
+        <f t="shared" si="1"/>
         <v>-727.55905511811022</v>
       </c>
     </row>
@@ -804,7 +804,7 @@
         <v>33.72</v>
       </c>
       <c r="C28" s="1">
-        <f>B28*sc</f>
+        <f t="shared" si="1"/>
         <v>1327.5590551181103</v>
       </c>
     </row>
@@ -817,7 +817,7 @@
         <v>-2.88</v>
       </c>
       <c r="C29" s="1">
-        <f>B29*sc</f>
+        <f t="shared" si="1"/>
         <v>-113.38582677165354</v>
       </c>
     </row>
@@ -830,7 +830,7 @@
         <v>18.12</v>
       </c>
       <c r="C30" s="1">
-        <f>B30*sc</f>
+        <f t="shared" si="1"/>
         <v>713.38582677165357</v>
       </c>
     </row>
@@ -844,7 +844,7 @@
         <v>0</v>
       </c>
       <c r="B33">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -852,7 +852,7 @@
         <v>8</v>
       </c>
       <c r="B34">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>16</v>
@@ -888,11 +888,11 @@
       </c>
       <c r="B37">
         <f>-B33/2</f>
-        <v>-12.5</v>
+        <v>-13</v>
       </c>
       <c r="C37" s="1">
         <f>B37*sc</f>
-        <v>-492.12598425196853</v>
+        <v>-511.81102362204729</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -901,11 +901,11 @@
       </c>
       <c r="B38">
         <f>B33/2</f>
-        <v>12.5</v>
+        <v>13</v>
       </c>
       <c r="C38" s="1">
         <f>B38*sc</f>
-        <v>492.12598425196853</v>
+        <v>511.81102362204729</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -914,11 +914,11 @@
       </c>
       <c r="B39">
         <f>-B34/2</f>
-        <v>-5.5</v>
+        <v>-6</v>
       </c>
       <c r="C39" s="1">
         <f>B39*sc</f>
-        <v>-216.53543307086613</v>
+        <v>-236.22047244094489</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -927,11 +927,11 @@
       </c>
       <c r="B40">
         <f>B34/2</f>
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="C40" s="1">
         <f>B40*sc</f>
-        <v>216.53543307086613</v>
+        <v>236.22047244094489</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -947,11 +947,11 @@
         <v>-11.43</v>
       </c>
       <c r="D41" s="1">
-        <f>B41*sc</f>
+        <f t="shared" ref="D41:E44" si="2">B41*sc</f>
         <v>50</v>
       </c>
       <c r="E41" s="1">
-        <f>C41*sc</f>
+        <f t="shared" si="2"/>
         <v>-450</v>
       </c>
     </row>
@@ -968,11 +968,11 @@
         <v>-11.43</v>
       </c>
       <c r="D42" s="1">
-        <f>B42*sc</f>
+        <f t="shared" si="2"/>
         <v>-50</v>
       </c>
       <c r="E42" s="1">
-        <f>C42*sc</f>
+        <f t="shared" si="2"/>
         <v>-450</v>
       </c>
     </row>
@@ -989,11 +989,11 @@
         <v>11.43</v>
       </c>
       <c r="D43" s="1">
-        <f>B43*sc</f>
+        <f t="shared" si="2"/>
         <v>50</v>
       </c>
       <c r="E43" s="1">
-        <f>C43*sc</f>
+        <f t="shared" si="2"/>
         <v>450</v>
       </c>
     </row>
@@ -1010,11 +1010,11 @@
         <v>11.43</v>
       </c>
       <c r="D44" s="1">
-        <f>B44*sc</f>
+        <f t="shared" si="2"/>
         <v>-50</v>
       </c>
       <c r="E44" s="1">
-        <f>C44*sc</f>
+        <f t="shared" si="2"/>
         <v>450</v>
       </c>
     </row>

</xml_diff>